<commit_message>
Add Employee Related changes
</commit_message>
<xml_diff>
--- a/OrangeHRM_POMFrameWork/TestData/OrangeHRMTestData.xlsx
+++ b/OrangeHRM_POMFrameWork/TestData/OrangeHRMTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="7935" windowWidth="20055" xWindow="240" yWindow="75"/>
+    <workbookView activeTab="2" windowHeight="7935" windowWidth="20055" xWindow="240" yWindow="75"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" r:id="rId1" sheetId="2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="57">
   <si>
     <t>Password</t>
   </si>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -625,6 +625,9 @@
       <c r="F3" t="s">
         <v>54</v>
       </c>
+      <c r="G3" t="s">
+        <v>55</v>
+      </c>
       <c r="H3" t="s">
         <v>50</v>
       </c>
@@ -707,6 +710,9 @@
       </c>
       <c r="F7" t="s">
         <v>54</v>
+      </c>
+      <c r="G7" t="s">
+        <v>56</v>
       </c>
       <c r="H7" t="s">
         <v>49</v>
@@ -986,23 +992,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="15.75" r="1" spans="1:7">
+    <row ht="15.75" r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1013,19 +1020,25 @@
         <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1036,19 +1049,25 @@
         <v>38</v>
       </c>
       <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1059,19 +1078,25 @@
         <v>39</v>
       </c>
       <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1082,15 +1107,21 @@
         <v>40</v>
       </c>
       <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>